<commit_message>
trackman score for exact distance matches
</commit_message>
<xml_diff>
--- a/TrackmanData/TestCenterAndCombineReportResults.xlsx
+++ b/TrackmanData/TestCenterAndCombineReportResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rehn/IdeaProjects/GCQuadCombineTest/TrackmanData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A4A81B-96BF-B047-9ABD-618006CC6A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310901D5-A14B-4B4A-9C14-81F41D135878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="520" windowWidth="64000" windowHeight="25080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="64000" windowHeight="25080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Pin absolute penalty point" sheetId="5" r:id="rId1"/>
@@ -27647,9 +27647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC5614-BCA1-4843-A31B-9FFACE729F12}">
   <dimension ref="A1:BS151"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AZ20" sqref="AZ20"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -48258,7 +48258,7 @@
   <dimension ref="A1:R111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:Q3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>